<commit_message>
Add `task-11` in `simulation-modeling`
</commit_message>
<xml_diff>
--- a/4-course-7-semester/simulation-modeling/task-10/SaveFigureExcel.xlsx
+++ b/4-course-7-semester/simulation-modeling/task-10/SaveFigureExcel.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="3">
   <si>
     <t>Прямоугольник</t>
   </si>
@@ -150,7 +150,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="n">
-        <v>9.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -280,10 +280,129 @@
         <v>430.0</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>125.0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>125.0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="n">
+        <v>125.0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>125.0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>200.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>200.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>175.0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>125.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>125.0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>175.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>175.0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>175.0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>